<commit_message>
reto superado en ga
</commit_message>
<xml_diff>
--- a/Lab 4/ GA.xlsx
+++ b/Lab 4/ GA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87CE63B-44DF-B149-AD20-99A0D5C42237}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C2A9A5-C09E-604B-9A12-8803EA07EEFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,7 +671,7 @@
   <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -759,31 +759,31 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>5.8104540000000003E-2</v>
+        <v>0.57518670000000005</v>
       </c>
       <c r="E4" s="2">
-        <v>1402712</v>
+        <v>1575331</v>
       </c>
       <c r="F4" s="2">
-        <v>62220.02</v>
+        <v>13232.5</v>
       </c>
       <c r="G4" s="2">
-        <v>12231.01</v>
+        <v>7468.1350000000002</v>
       </c>
       <c r="H4" s="2">
-        <v>679.14700000000005</v>
+        <v>1377.499</v>
       </c>
       <c r="I4" s="2">
-        <v>3.0077389999999999</v>
+        <v>2.0710200000000002E-2</v>
       </c>
       <c r="J4" s="2">
-        <v>20.347079999999998</v>
+        <v>20.951460000000001</v>
       </c>
       <c r="K4" s="2">
-        <v>102.9357</v>
+        <v>26.56195</v>
       </c>
       <c r="L4" s="2">
-        <v>337.68439999999998</v>
+        <v>56.065860000000001</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
@@ -804,19 +804,19 @@
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>62220.02</v>
+        <v>13232.5</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>12231.01</v>
+        <v>7468.1350000000002</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>679.14700000000005</v>
+        <v>1377.499</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
-        <v>3.0077389999999999</v>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
@@ -824,11 +824,11 @@
       </c>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>102.9357</v>
+        <v>26.56195</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>337.68439999999998</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -900,19 +900,19 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>4.3715832942515928E-3</v>
+        <v>2.0555450595125639E-2</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>1.1119277966414876E-2</v>
+        <v>1.8210704546717485E-2</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
-        <v>4.6823441758558897E-2</v>
+        <v>2.3085316214385636E-2</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="1"/>
-        <v>1.768770495046279E-2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
@@ -920,15 +920,15 @@
       </c>
       <c r="K9" s="5">
         <f t="shared" si="1"/>
-        <v>0.11852059100972742</v>
+        <v>0.45930362793394308</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="1"/>
-        <v>0.43531771085664606</v>
+        <v>1</v>
       </c>
       <c r="M9" s="5">
         <f>SUM(C9:L9)</f>
-        <v>3.6338403098360614</v>
+        <v>5.5211550992901728</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -941,11 +941,11 @@
       </c>
       <c r="D10" s="5">
         <f t="shared" si="1"/>
-        <v>1.7139982300884958E-3</v>
+        <v>1.6967159292035402E-2</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>0.21883182527301093</v>
+        <v>0.24576146645865835</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
@@ -961,11 +961,11 @@
       </c>
       <c r="I10" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.38928947368421057</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="1"/>
-        <v>0.96890857142857134</v>
+        <v>0.99768857142857148</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="1"/>
@@ -973,11 +973,11 @@
       </c>
       <c r="L10" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.38140040816326531</v>
       </c>
       <c r="M10" s="5">
         <f>SUM(C10:L10)</f>
-        <v>7.1894543949316709</v>
+        <v>6.0311070790267411</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>